<commit_message>
add work dowload button
</commit_message>
<xml_diff>
--- a/1.Data/2.shiny/tar_edges.xlsx
+++ b/1.Data/2.shiny/tar_edges.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t xml:space="preserve">from_l</t>
   </si>
@@ -32,13 +32,13 @@
     <t xml:space="preserve">dashes</t>
   </si>
   <si>
-    <t xml:space="preserve">download_Copy.of.quotes_agregation_level11.xlsx</t>
+    <t xml:space="preserve">download_quotes_agregation_level1.xlsx</t>
   </si>
   <si>
     <t xml:space="preserve">download_files</t>
   </si>
   <si>
-    <t xml:space="preserve">12</t>
+    <t xml:space="preserve">4</t>
   </si>
   <si>
     <t xml:space="preserve">stem</t>
@@ -47,24 +47,12 @@
     <t xml:space="preserve">3</t>
   </si>
   <si>
-    <t xml:space="preserve">download_quotes_agregation_level1.xlsx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4</t>
-  </si>
-  <si>
     <t xml:space="preserve">download_quotes_agregation_level10.xlsx</t>
   </si>
   <si>
     <t xml:space="preserve">11</t>
   </si>
   <si>
-    <t xml:space="preserve">download_quotes_agregation_level11.xlsx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13</t>
-  </si>
-  <si>
     <t xml:space="preserve">download_quotes_agregation_level2.xlsx</t>
   </si>
   <si>
@@ -77,22 +65,22 @@
     <t xml:space="preserve">6</t>
   </si>
   <si>
+    <t xml:space="preserve">model_data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model_graph</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modelGraph</t>
+  </si>
+  <si>
     <t xml:space="preserve">downloadQuotes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">model_data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">model_graph</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">modelGraph</t>
   </si>
   <si>
     <t xml:space="preserve">quotes_forecast</t>
@@ -568,16 +556,16 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
@@ -585,19 +573,15 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7"/>
+      <c r="D7"/>
+      <c r="E7" t="s">
         <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" t="s">
-        <v>10</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
@@ -605,7 +589,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
@@ -621,19 +605,19 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>23</v>
       </c>
       <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
         <v>24</v>
-      </c>
-      <c r="D9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" t="s">
-        <v>25</v>
       </c>
       <c r="F9" t="b">
         <v>0</v>
@@ -641,7 +625,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
         <v>23</v>
@@ -649,7 +633,7 @@
       <c r="C10"/>
       <c r="D10"/>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F10" t="b">
         <v>0</v>
@@ -657,15 +641,15 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C11"/>
       <c r="D11"/>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F11" t="b">
         <v>0</v>
@@ -673,19 +657,19 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
         <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="D12" t="s">
         <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F12" t="b">
         <v>0</v>
@@ -693,15 +677,19 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
         <v>27</v>
       </c>
-      <c r="C13"/>
-      <c r="D13"/>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
       <c r="E13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F13" t="b">
         <v>0</v>
@@ -709,15 +697,19 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14"/>
-      <c r="D14"/>
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
       <c r="E14" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="F14" t="b">
         <v>0</v>
@@ -728,16 +720,12 @@
         <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" t="s">
-        <v>9</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C15"/>
+      <c r="D15"/>
       <c r="E15" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F15" t="b">
         <v>0</v>
@@ -748,16 +736,12 @@
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" t="s">
-        <v>9</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="C16"/>
+      <c r="D16"/>
       <c r="E16" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="F16" t="b">
         <v>0</v>
@@ -765,19 +749,19 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
         <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D17" t="s">
         <v>9</v>
       </c>
       <c r="E17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F17" t="b">
         <v>0</v>
@@ -785,7 +769,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" t="s">
         <v>31</v>
@@ -793,7 +777,7 @@
       <c r="C18"/>
       <c r="D18"/>
       <c r="E18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F18" t="b">
         <v>0</v>
@@ -801,15 +785,19 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19"/>
-      <c r="D19"/>
+        <v>31</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
+        <v>9</v>
+      </c>
       <c r="E19" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="F19" t="b">
         <v>0</v>
@@ -817,15 +805,19 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20"/>
-      <c r="D20"/>
+        <v>31</v>
+      </c>
+      <c r="C20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
       <c r="E20" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="F20" t="b">
         <v>0</v>
@@ -833,19 +825,19 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" t="s">
         <v>32</v>
-      </c>
-      <c r="D21" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" t="s">
-        <v>36</v>
       </c>
       <c r="F21" t="b">
         <v>0</v>
@@ -853,15 +845,19 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22"/>
-      <c r="D22"/>
+        <v>31</v>
+      </c>
+      <c r="C22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" t="s">
+        <v>9</v>
+      </c>
       <c r="E22" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F22" t="b">
         <v>0</v>
@@ -869,19 +865,19 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C23" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D23" t="s">
         <v>9</v>
       </c>
       <c r="E23" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F23" t="b">
         <v>0</v>
@@ -892,16 +888,12 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" t="s">
-        <v>9</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C24"/>
+      <c r="D24"/>
       <c r="E24" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="F24" t="b">
         <v>0</v>
@@ -909,19 +901,15 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="B25" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25" t="s">
-        <v>9</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="C25"/>
+      <c r="D25"/>
       <c r="E25" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F25" t="b">
         <v>0</v>
@@ -929,19 +917,19 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B26" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C26" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" t="s">
         <v>28</v>
-      </c>
-      <c r="D26" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" t="s">
-        <v>36</v>
       </c>
       <c r="F26" t="b">
         <v>0</v>
@@ -949,19 +937,15 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" t="s">
-        <v>33</v>
-      </c>
-      <c r="D27" t="s">
-        <v>9</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C27"/>
+      <c r="D27"/>
       <c r="E27" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="F27" t="b">
         <v>0</v>
@@ -969,89 +953,21 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28"/>
-      <c r="D28"/>
+        <v>17</v>
+      </c>
+      <c r="C28" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" t="s">
+        <v>9</v>
+      </c>
       <c r="E28" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F28" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29"/>
-      <c r="D29"/>
-      <c r="E29" t="s">
-        <v>32</v>
-      </c>
-      <c r="F29" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="s">
-        <v>22</v>
-      </c>
-      <c r="B30" t="s">
-        <v>30</v>
-      </c>
-      <c r="C30" t="s">
-        <v>24</v>
-      </c>
-      <c r="D30" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" t="s">
-        <v>32</v>
-      </c>
-      <c r="F30" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="s">
-        <v>39</v>
-      </c>
-      <c r="B31" t="s">
-        <v>22</v>
-      </c>
-      <c r="C31"/>
-      <c r="D31"/>
-      <c r="E31" t="s">
-        <v>24</v>
-      </c>
-      <c r="F31" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="s">
-        <v>27</v>
-      </c>
-      <c r="B32" t="s">
-        <v>22</v>
-      </c>
-      <c r="C32" t="s">
-        <v>28</v>
-      </c>
-      <c r="D32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E32" t="s">
-        <v>24</v>
-      </c>
-      <c r="F32" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>